<commit_message>
Fixed CDS files tab function
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1D6085-481A-418D-9F0A-ED42CE8C1EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E00391-C67A-4992-B251-967253C6F03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -95,22 +95,6 @@
     <t>MATCH (s:study)&lt;--(p:participant)
 WHERE s.study_name in ["GECCO OICR: Molecular Pathological Epidemiology of Colorectal Cancer"]
 OPTIONAL MATCH (p)&lt;--(samp:sample)
-OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
-OPTIONAL MATCH (samp)&lt;--(f:file)
-WITH DISTINCT samp,diag,s,p
-RETURN  
- coalesce(samp.sample_id, '') as `Sample ID`,
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(samp.sample_tumor_status,'') as `Tumor`,
-coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id LIMIT 100</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE s.study_name in ["GECCO OICR: Molecular Pathological Epidemiology of Colorectal Cancer"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
 WITH p, s, collect(distinct samp.sample_id) as samp
 RETURN   
  coalesce(p.participant_id,'') as `Participant ID`,
@@ -119,6 +103,19 @@
  coalesce(p.gender,'') as `Gender`,
  coalesce(apoc.text.join(samp, ','), '') as `Samples`
  ORDER By p.participant_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
+WHERE s.study_name in ["GECCO OICR: Molecular Pathological Epidemiology of Colorectal Cancer"]
+WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
+RETURN  
+ coalesce(samp.sample_id, '') as `Sample ID`,
+ coalesce(p.participant_id,'') as `Participant ID`,
+ coalesce(s.study_name, '') as `Study Name`,
+ coalesce(s.phs_accession,'') as `Accession`,
+ coalesce(tumor,'') as `Tumor`,
+coalesce(samp.sample_type,'') as `Analyte Type`
+ORDER By samp.sample_id LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -501,7 +498,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +532,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>10</v>
@@ -547,12 +544,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="249.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
fix CDS read table function
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Desktop\Sowjanya\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E00391-C67A-4992-B251-967253C6F03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8957C0F-2C1C-49DC-94AB-D6D2CFB52F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -113,9 +113,9 @@
  coalesce(p.participant_id,'') as `Participant ID`,
  coalesce(s.study_name, '') as `Study Name`,
  coalesce(s.phs_accession,'') as `Accession`,
- coalesce(tumor,'') as `Tumor`,
+ coalesce(samp.sample_tumor_status,'') as `Tumor`,
 coalesce(samp.sample_type,'') as `Analyte Type`
-ORDER By samp.sample_id LIMIT 100</t>
+  ORDER By samp.sample_id LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Filter - Study - Test Suit
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Desktop\Sowjanya\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\CDS Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8957C0F-2C1C-49DC-94AB-D6D2CFB52F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DCC9EB-17D4-402F-8F2F-20B72C3B0295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>TabName</t>
   </si>
   <si>
-    <t>CasesTab</t>
-  </si>
-  <si>
     <t>SamplesTab</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
  coalesce(samp.sample_tumor_status,'') as `Tumor`,
 coalesce(samp.sample_type,'') as `Analyte Type`
   ORDER By samp.sample_id LIMIT 100</t>
+  </si>
+  <si>
+    <t>ParticipantsTab</t>
   </si>
 </sst>
 </file>
@@ -498,19 +498,19 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.21875" customWidth="1"/>
-    <col min="5" max="5" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.28515625" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -527,62 +527,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="189" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="218.4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CDS Study filter fixes
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
+++ b/InputFiles/TC01_CDS_Filter_Study-GECCO-OICR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\CDS Automation\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0717new\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DCC9EB-17D4-402F-8F2F-20B72C3B0295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16964E35-4300-4BEC-9C0A-8054A8B17272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -89,19 +89,6 @@
    ORDER By f.file_name LIMIT 100</t>
   </si>
   <si>
-    <t>MATCH (s:study)&lt;--(p:participant)
-WHERE s.study_name in ["GECCO OICR: Molecular Pathological Epidemiology of Colorectal Cancer"]
-OPTIONAL MATCH (p)&lt;--(samp:sample)
-WITH p, s, collect(distinct samp.sample_id) as samp
-RETURN   
- coalesce(p.participant_id,'') as `Participant ID`,
- coalesce(s.study_name, '') as `Study Name`,
- coalesce(s.phs_accession,'') as `Accession`,
- coalesce(p.gender,'') as `Gender`,
- coalesce(apoc.text.join(samp, ','), '') as `Samples`
- ORDER By p.participant_id LIMIT 100</t>
-  </si>
-  <si>
     <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
 WHERE s.study_name in ["GECCO OICR: Molecular Pathological Epidemiology of Colorectal Cancer"]
 WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
@@ -116,6 +103,26 @@
   </si>
   <si>
     <t>ParticipantsTab</t>
+  </si>
+  <si>
+    <t>MATCH (p:participant)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp)&lt;--(f:file)
+OPTIONAL MATCH (f)&lt;--(g:genomic_info)
+WITH s, p, samp, f, g, diag
+WHERE s.study_name in ["GECCO OICR: Molecular Pathological Epidemiology of Colorectal Cancer"]
+OPTIONAL MATCH (p)--&gt;(s:study)
+OPTIONAL MATCH (samp:sample)--&gt;(p)
+WITH s, p, apoc.coll.sort(collect(distinct samp.sample_id)) as samp
+RETURN 
+coalesce(p.participant_id,'') as `Participant ID`,
+coalesce(s.study_name, '') as `Study Name`,
+coalesce(s.phs_accession,'') as `Accession`,
+coalesce(p.gender,'') as `Gender`,
+coalesce(apoc.text.join(samp, ','), '') as `Samples`
+ORDER BY p.participant_id
+LIMIT 100</t>
   </si>
 </sst>
 </file>
@@ -498,7 +505,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,12 +534,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="189" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>9</v>
@@ -549,7 +556,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>

</xml_diff>